<commit_message>
converted dates to numeric + created working script
</commit_message>
<xml_diff>
--- a/data/arabidopsis_data.xlsx
+++ b/data/arabidopsis_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nineluijendijk/evolutionarybiology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FB0F6A-144F-404F-B8C0-42963605F667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE69859-4589-DB46-8F46-1730AC25CD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d\.m"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -225,16 +225,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,8 +454,8 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L61" sqref="L61"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -468,7 +467,7 @@
     <col min="8" max="16384" width="12.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -484,7 +483,7 @@
       <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -500,15 +499,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
-        <v>44989</v>
+      <c r="C2" s="7">
+        <v>4.3</v>
       </c>
       <c r="D2" s="3">
         <v>8</v>
@@ -516,8 +515,8 @@
       <c r="E2" s="3">
         <v>28</v>
       </c>
-      <c r="F2" s="5">
-        <v>45116</v>
+      <c r="F2" s="7">
+        <v>9.6999999999999993</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -529,14 +528,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>8</v>
       </c>
       <c r="D3" s="3">
@@ -545,8 +544,8 @@
       <c r="E3" s="3">
         <v>27</v>
       </c>
-      <c r="F3" s="5">
-        <v>45055</v>
+      <c r="F3" s="7">
+        <v>9.5</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
@@ -559,14 +558,14 @@
       </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>2</v>
       </c>
       <c r="D4" s="3">
@@ -575,8 +574,8 @@
       <c r="E4" s="3">
         <v>12</v>
       </c>
-      <c r="F4" s="5">
-        <v>45025</v>
+      <c r="F4" s="7">
+        <v>9.4</v>
       </c>
       <c r="G4" s="3">
         <v>2</v>
@@ -588,15 +587,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="5">
-        <v>44929</v>
+      <c r="C5" s="7">
+        <v>3.1</v>
       </c>
       <c r="D5" s="3">
         <v>5</v>
@@ -604,8 +603,8 @@
       <c r="E5" s="3">
         <v>12</v>
       </c>
-      <c r="F5" s="5">
-        <v>45113</v>
+      <c r="F5" s="7">
+        <v>6.7</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -617,15 +616,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="5">
-        <v>45050</v>
+      <c r="C6" s="7">
+        <v>4.5</v>
       </c>
       <c r="D6" s="3">
         <v>7</v>
@@ -633,8 +632,8 @@
       <c r="E6" s="3">
         <v>22</v>
       </c>
-      <c r="F6" s="5">
-        <v>44996</v>
+      <c r="F6" s="7">
+        <v>11.3</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -647,15 +646,15 @@
       </c>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="5">
-        <v>45175</v>
+      <c r="C7" s="7">
+        <v>6.9</v>
       </c>
       <c r="D7" s="3">
         <v>10</v>
@@ -663,8 +662,8 @@
       <c r="E7" s="3">
         <v>35</v>
       </c>
-      <c r="F7" s="5">
-        <v>45117</v>
+      <c r="F7" s="7">
+        <v>10.7</v>
       </c>
       <c r="G7" s="3">
         <v>2</v>
@@ -676,15 +675,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="5">
-        <v>45050</v>
+      <c r="C8" s="7">
+        <v>4.5</v>
       </c>
       <c r="D8" s="3">
         <v>9</v>
@@ -692,8 +691,8 @@
       <c r="E8" s="3">
         <v>40</v>
       </c>
-      <c r="F8" s="5">
-        <v>44967</v>
+      <c r="F8" s="7">
+        <v>10.199999999999999</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -705,15 +704,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="5">
-        <v>44928</v>
+      <c r="C9" s="7">
+        <v>2.1</v>
       </c>
       <c r="D9" s="3">
         <v>6</v>
@@ -721,8 +720,8 @@
       <c r="E9" s="3">
         <v>23</v>
       </c>
-      <c r="F9" s="5">
-        <v>45147</v>
+      <c r="F9" s="7">
+        <v>9.8000000000000007</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -734,14 +733,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>0.8</v>
       </c>
       <c r="D10" s="3">
@@ -750,8 +749,8 @@
       <c r="E10" s="3">
         <v>20</v>
       </c>
-      <c r="F10" s="5">
-        <v>45087</v>
+      <c r="F10" s="7">
+        <v>10.6</v>
       </c>
       <c r="G10" s="3">
         <v>2</v>
@@ -763,15 +762,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="5">
-        <v>45140</v>
+      <c r="C11" s="7">
+        <v>2.8</v>
       </c>
       <c r="D11" s="3">
         <v>8</v>
@@ -779,8 +778,8 @@
       <c r="E11" s="3">
         <v>25</v>
       </c>
-      <c r="F11" s="5">
-        <v>45054</v>
+      <c r="F11" s="7">
+        <v>8.5</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
@@ -793,15 +792,15 @@
       </c>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
-      <c r="C12" s="5">
-        <v>45143</v>
+      <c r="C12" s="7">
+        <v>5.8</v>
       </c>
       <c r="D12" s="3">
         <v>11</v>
@@ -809,7 +808,7 @@
       <c r="E12" s="3">
         <v>23</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="7">
         <v>10</v>
       </c>
       <c r="G12" s="3">
@@ -822,15 +821,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
       </c>
-      <c r="C13" s="5">
-        <v>45112</v>
+      <c r="C13" s="7">
+        <v>5.7</v>
       </c>
       <c r="D13" s="3">
         <v>12</v>
@@ -838,7 +837,7 @@
       <c r="E13" s="3">
         <v>30</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="7">
         <v>7</v>
       </c>
       <c r="G13" s="3">
@@ -852,15 +851,15 @@
       </c>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="3">
         <v>3</v>
       </c>
-      <c r="C14" s="5">
-        <v>45112</v>
+      <c r="C14" s="7">
+        <v>5.7</v>
       </c>
       <c r="D14" s="3">
         <v>15</v>
@@ -868,8 +867,8 @@
       <c r="E14" s="3">
         <v>30</v>
       </c>
-      <c r="F14" s="5">
-        <v>45026</v>
+      <c r="F14" s="7">
+        <v>10.4</v>
       </c>
       <c r="G14" s="3">
         <v>2</v>
@@ -882,15 +881,15 @@
       </c>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>4</v>
       </c>
-      <c r="C15" s="5">
-        <v>45145</v>
+      <c r="C15" s="7">
+        <v>7.8</v>
       </c>
       <c r="D15" s="3">
         <v>14</v>
@@ -898,8 +897,8 @@
       <c r="E15" s="3">
         <v>44</v>
       </c>
-      <c r="F15" s="5">
-        <v>45117</v>
+      <c r="F15" s="7">
+        <v>10.7</v>
       </c>
       <c r="G15" s="3">
         <v>2</v>
@@ -912,15 +911,15 @@
       </c>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="3">
         <v>5</v>
       </c>
-      <c r="C16" s="5">
-        <v>45050</v>
+      <c r="C16" s="7">
+        <v>4.5</v>
       </c>
       <c r="D16" s="3">
         <v>18</v>
@@ -928,8 +927,8 @@
       <c r="E16" s="3">
         <v>42</v>
       </c>
-      <c r="F16" s="5">
-        <v>45144</v>
+      <c r="F16" s="7">
+        <v>6.8</v>
       </c>
       <c r="G16" s="3">
         <v>2</v>
@@ -942,14 +941,14 @@
       </c>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3">
         <v>6</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="7">
         <v>1</v>
       </c>
       <c r="D17" s="3">
@@ -958,8 +957,8 @@
       <c r="E17" s="3">
         <v>15</v>
       </c>
-      <c r="F17" s="5">
-        <v>45049</v>
+      <c r="F17" s="7">
+        <v>3.5</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
@@ -972,15 +971,15 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="3">
         <v>7</v>
       </c>
-      <c r="C18" s="5">
-        <v>45020</v>
+      <c r="C18" s="7">
+        <v>4.4000000000000004</v>
       </c>
       <c r="D18" s="3">
         <v>15</v>
@@ -988,7 +987,7 @@
       <c r="E18" s="3">
         <v>42</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="7">
         <v>9</v>
       </c>
       <c r="G18" s="3">
@@ -1001,15 +1000,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="3">
         <v>8</v>
       </c>
-      <c r="C19" s="5">
-        <v>44963</v>
+      <c r="C19" s="7">
+        <v>6.2</v>
       </c>
       <c r="D19" s="3">
         <v>12</v>
@@ -1017,8 +1016,8 @@
       <c r="E19" s="3">
         <v>33</v>
       </c>
-      <c r="F19" s="5">
-        <v>45054</v>
+      <c r="F19" s="7">
+        <v>8.5</v>
       </c>
       <c r="G19" s="3">
         <v>3</v>
@@ -1031,15 +1030,15 @@
       </c>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="3">
         <v>9</v>
       </c>
-      <c r="C20" s="5">
-        <v>44930</v>
+      <c r="C20" s="7">
+        <v>4.0999999999999996</v>
       </c>
       <c r="D20" s="3">
         <v>9</v>
@@ -1047,7 +1046,7 @@
       <c r="E20" s="3">
         <v>23</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="7">
         <v>11</v>
       </c>
       <c r="G20" s="3">
@@ -1060,15 +1059,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="3">
         <v>10</v>
       </c>
-      <c r="C21" s="5">
-        <v>45175</v>
+      <c r="C21" s="7">
+        <v>6.9</v>
       </c>
       <c r="D21" s="3">
         <v>10</v>
@@ -1076,8 +1075,8 @@
       <c r="E21" s="3">
         <v>32</v>
       </c>
-      <c r="F21" s="5">
-        <v>44996</v>
+      <c r="F21" s="7">
+        <v>11.3</v>
       </c>
       <c r="G21" s="3">
         <v>2</v>
@@ -1089,15 +1088,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
       </c>
-      <c r="C22" s="5">
-        <v>44959</v>
+      <c r="C22" s="7">
+        <v>2.2000000000000002</v>
       </c>
       <c r="D22" s="3">
         <v>8</v>
@@ -1105,8 +1104,8 @@
       <c r="E22" s="3">
         <v>38</v>
       </c>
-      <c r="F22" s="5">
-        <v>45055</v>
+      <c r="F22" s="7">
+        <v>9.5</v>
       </c>
       <c r="G22" s="3">
         <v>2</v>
@@ -1118,15 +1117,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="3">
         <v>2</v>
       </c>
-      <c r="C23" s="5">
-        <v>45141</v>
+      <c r="C23" s="7">
+        <v>3.8</v>
       </c>
       <c r="D23" s="3">
         <v>7</v>
@@ -1134,8 +1133,8 @@
       <c r="E23" s="3">
         <v>22</v>
       </c>
-      <c r="F23" s="5">
-        <v>45023</v>
+      <c r="F23" s="7">
+        <v>7.4</v>
       </c>
       <c r="G23" s="3">
         <v>2</v>
@@ -1147,15 +1146,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="3">
         <v>3</v>
       </c>
-      <c r="C24" s="5">
-        <v>45083</v>
+      <c r="C24" s="7">
+        <v>6.6</v>
       </c>
       <c r="D24" s="3">
         <v>13</v>
@@ -1163,8 +1162,8 @@
       <c r="E24" s="3">
         <v>48</v>
       </c>
-      <c r="F24" s="5">
-        <v>45027</v>
+      <c r="F24" s="7">
+        <v>11.4</v>
       </c>
       <c r="G24" s="3">
         <v>3</v>
@@ -1176,21 +1175,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="3">
         <v>4</v>
       </c>
-      <c r="C25" s="5">
-        <v>45051</v>
+      <c r="C25" s="7">
+        <v>5.5</v>
       </c>
       <c r="E25" s="3">
         <v>64</v>
       </c>
-      <c r="F25" s="5">
-        <v>45055</v>
+      <c r="F25" s="7">
+        <v>9.5</v>
       </c>
       <c r="G25" s="3">
         <v>3</v>
@@ -1203,15 +1202,15 @@
       </c>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="3">
         <v>5</v>
       </c>
-      <c r="C26" s="5">
-        <v>45079</v>
+      <c r="C26" s="7">
+        <v>2.6</v>
       </c>
       <c r="D26" s="3">
         <v>7</v>
@@ -1219,8 +1218,8 @@
       <c r="E26" s="3">
         <v>24</v>
       </c>
-      <c r="F26" s="5">
-        <v>45087</v>
+      <c r="F26" s="7">
+        <v>10.6</v>
       </c>
       <c r="G26" s="3">
         <v>2</v>
@@ -1232,15 +1231,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="3">
         <v>6</v>
       </c>
-      <c r="C27" s="5">
-        <v>44931</v>
+      <c r="C27" s="7">
+        <v>5.0999999999999996</v>
       </c>
       <c r="D27" s="3">
         <v>11</v>
@@ -1248,8 +1247,8 @@
       <c r="E27" s="3">
         <v>34</v>
       </c>
-      <c r="F27" s="5">
-        <v>45058</v>
+      <c r="F27" s="7">
+        <v>12.5</v>
       </c>
       <c r="G27" s="3">
         <v>2</v>
@@ -1261,15 +1260,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="3">
         <v>7</v>
       </c>
-      <c r="C28" s="5">
-        <v>45018</v>
+      <c r="C28" s="7">
+        <v>2.4</v>
       </c>
       <c r="D28" s="3">
         <v>7</v>
@@ -1277,7 +1276,7 @@
       <c r="E28" s="3">
         <v>24</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="7">
         <v>8</v>
       </c>
       <c r="G28" s="3">
@@ -1290,15 +1289,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="5">
-        <v>44961</v>
+      <c r="C29" s="7">
+        <v>4.2</v>
       </c>
       <c r="D29" s="3">
         <v>10</v>
@@ -1306,7 +1305,7 @@
       <c r="E29" s="3">
         <v>32</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="7">
         <v>6</v>
       </c>
       <c r="G29" s="3">
@@ -1319,15 +1318,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="3">
         <v>2</v>
       </c>
-      <c r="C30" s="5">
-        <v>45081</v>
+      <c r="C30" s="7">
+        <v>4.5999999999999996</v>
       </c>
       <c r="D30" s="3">
         <v>17</v>
@@ -1335,8 +1334,8 @@
       <c r="E30" s="3">
         <v>68</v>
       </c>
-      <c r="F30" s="5">
-        <v>45055</v>
+      <c r="F30" s="7">
+        <v>9.5</v>
       </c>
       <c r="G30" s="3">
         <v>3</v>
@@ -1348,15 +1347,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="3">
         <v>3</v>
       </c>
-      <c r="C31" s="5">
-        <v>45080</v>
+      <c r="C31" s="7">
+        <v>3.6</v>
       </c>
       <c r="D31" s="3">
         <v>9</v>
@@ -1364,8 +1363,8 @@
       <c r="E31" s="3">
         <v>18</v>
       </c>
-      <c r="F31" s="5">
-        <v>45116</v>
+      <c r="F31" s="7">
+        <v>9.6999999999999993</v>
       </c>
       <c r="G31" s="3">
         <v>2</v>
@@ -1377,15 +1376,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="3">
         <v>4</v>
       </c>
-      <c r="C32" s="5">
-        <v>44992</v>
+      <c r="C32" s="7">
+        <v>7.3</v>
       </c>
       <c r="D32" s="3">
         <v>12</v>
@@ -1393,8 +1392,8 @@
       <c r="E32" s="3">
         <v>36</v>
       </c>
-      <c r="F32" s="5">
-        <v>45028</v>
+      <c r="F32" s="7">
+        <v>12.4</v>
       </c>
       <c r="G32" s="3">
         <v>3</v>
@@ -1406,15 +1405,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="3">
         <v>5</v>
       </c>
-      <c r="C33" s="5">
-        <v>45082</v>
+      <c r="C33" s="7">
+        <v>5.6</v>
       </c>
       <c r="D33" s="3">
         <v>9</v>
@@ -1422,8 +1421,8 @@
       <c r="E33" s="3">
         <v>24</v>
       </c>
-      <c r="F33" s="5">
-        <v>45117</v>
+      <c r="F33" s="7">
+        <v>10.7</v>
       </c>
       <c r="G33" s="3">
         <v>2</v>
@@ -1435,15 +1434,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="3">
         <v>6</v>
       </c>
-      <c r="C34" s="5">
-        <v>45020</v>
+      <c r="C34" s="7">
+        <v>4.4000000000000004</v>
       </c>
       <c r="D34" s="3">
         <v>12</v>
@@ -1451,7 +1450,7 @@
       <c r="E34" s="3">
         <v>32</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="7">
         <v>10</v>
       </c>
       <c r="G34" s="3">
@@ -1464,15 +1463,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B35" s="3">
         <v>7</v>
       </c>
-      <c r="C35" s="5">
-        <v>45172</v>
+      <c r="C35" s="7">
+        <v>3.9</v>
       </c>
       <c r="D35" s="3">
         <v>13</v>
@@ -1480,8 +1479,8 @@
       <c r="E35" s="3">
         <v>54</v>
       </c>
-      <c r="F35" s="5">
-        <v>44934</v>
+      <c r="F35" s="7">
+        <v>8.1</v>
       </c>
       <c r="G35" s="3">
         <v>2</v>
@@ -1493,15 +1492,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B36" s="3">
         <v>8</v>
       </c>
-      <c r="C36" s="5">
-        <v>45113</v>
+      <c r="C36" s="7">
+        <v>6.7</v>
       </c>
       <c r="D36" s="3">
         <v>11</v>
@@ -1509,8 +1508,8 @@
       <c r="E36" s="3">
         <v>32</v>
       </c>
-      <c r="F36" s="5">
-        <v>45055</v>
+      <c r="F36" s="7">
+        <v>9.5</v>
       </c>
       <c r="G36" s="3">
         <v>2</v>
@@ -1522,15 +1521,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
       </c>
-      <c r="C37" s="5">
-        <v>45081</v>
+      <c r="C37" s="7">
+        <v>4.5999999999999996</v>
       </c>
       <c r="D37" s="3">
         <v>13</v>
@@ -1538,8 +1537,8 @@
       <c r="E37" s="3">
         <v>82</v>
       </c>
-      <c r="F37" s="5">
-        <v>45084</v>
+      <c r="F37" s="7">
+        <v>7.6</v>
       </c>
       <c r="G37" s="3">
         <v>3</v>
@@ -1551,15 +1550,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="3">
         <v>2</v>
       </c>
-      <c r="C38" s="5">
-        <v>45085</v>
+      <c r="C38" s="7">
+        <v>8.6</v>
       </c>
       <c r="D38" s="3">
         <v>15</v>
@@ -1567,8 +1566,8 @@
       <c r="E38" s="3">
         <v>31</v>
       </c>
-      <c r="F38" s="5">
-        <v>45025</v>
+      <c r="F38" s="7">
+        <v>9.4</v>
       </c>
       <c r="G38" s="3">
         <v>4</v>
@@ -1581,15 +1580,15 @@
       </c>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="3">
         <v>3</v>
       </c>
-      <c r="C39" s="5">
-        <v>44991</v>
+      <c r="C39" s="7">
+        <v>6.3</v>
       </c>
       <c r="D39" s="3">
         <v>10</v>
@@ -1597,8 +1596,8 @@
       <c r="E39" s="3">
         <v>37</v>
       </c>
-      <c r="F39" s="5">
-        <v>45116</v>
+      <c r="F39" s="7">
+        <v>9.6999999999999993</v>
       </c>
       <c r="G39" s="3">
         <v>3</v>
@@ -1610,14 +1609,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B40" s="3">
         <v>4</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="7">
         <v>5</v>
       </c>
       <c r="D40" s="3">
@@ -1626,8 +1625,8 @@
       <c r="E40" s="3">
         <v>106</v>
       </c>
-      <c r="F40" s="5">
-        <v>45053</v>
+      <c r="F40" s="7">
+        <v>7.5</v>
       </c>
       <c r="G40" s="3">
         <v>3</v>
@@ -1642,14 +1641,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="3">
         <v>5</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="7">
         <v>5</v>
       </c>
       <c r="D41" s="3">
@@ -1658,8 +1657,8 @@
       <c r="E41" s="3">
         <v>34</v>
       </c>
-      <c r="F41" s="5">
-        <v>44967</v>
+      <c r="F41" s="7">
+        <v>10.199999999999999</v>
       </c>
       <c r="G41" s="3">
         <v>4</v>
@@ -1672,14 +1671,14 @@
       </c>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B42" s="3">
         <v>6</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="7">
         <v>6</v>
       </c>
       <c r="D42" s="3">
@@ -1688,7 +1687,7 @@
       <c r="E42" s="3">
         <v>70</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="7">
         <v>10</v>
       </c>
       <c r="G42" s="3">
@@ -1702,15 +1701,15 @@
       </c>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B43" s="3">
         <v>7</v>
       </c>
-      <c r="C43" s="5">
-        <v>45112</v>
+      <c r="C43" s="7">
+        <v>5.7</v>
       </c>
       <c r="D43" s="3">
         <v>25</v>
@@ -1718,8 +1717,8 @@
       <c r="E43" s="3">
         <v>98</v>
       </c>
-      <c r="F43" s="5">
-        <v>44993</v>
+      <c r="F43" s="7">
+        <v>8.3000000000000007</v>
       </c>
       <c r="G43" s="3">
         <v>4</v>
@@ -1732,14 +1731,14 @@
       </c>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B44" s="3">
         <v>8</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="7">
         <v>4</v>
       </c>
       <c r="D44" s="3">
@@ -1748,8 +1747,8 @@
       <c r="E44" s="3">
         <v>34</v>
       </c>
-      <c r="F44" s="5">
-        <v>45178</v>
+      <c r="F44" s="7">
+        <v>9.9</v>
       </c>
       <c r="G44" s="3">
         <v>4</v>
@@ -1761,15 +1760,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B45" s="3">
         <v>9</v>
       </c>
-      <c r="C45" s="5">
-        <v>45082</v>
+      <c r="C45" s="7">
+        <v>5.6</v>
       </c>
       <c r="D45" s="3">
         <v>8</v>
@@ -1777,8 +1776,8 @@
       <c r="E45" s="3">
         <v>70</v>
       </c>
-      <c r="F45" s="5">
-        <v>44937</v>
+      <c r="F45" s="7">
+        <v>11.1</v>
       </c>
       <c r="G45" s="3">
         <v>3</v>
@@ -1793,15 +1792,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B46" s="3">
         <v>1</v>
       </c>
-      <c r="C46" s="5">
-        <v>44931</v>
+      <c r="C46" s="7">
+        <v>5.0999999999999996</v>
       </c>
       <c r="D46" s="3">
         <v>27</v>
@@ -1809,8 +1808,8 @@
       <c r="E46" s="3">
         <v>98</v>
       </c>
-      <c r="F46" s="5">
-        <v>44965</v>
+      <c r="F46" s="7">
+        <v>8.1999999999999993</v>
       </c>
       <c r="G46" s="3">
         <v>3</v>
@@ -1822,15 +1821,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B47" s="3">
         <v>2</v>
       </c>
-      <c r="C47" s="5">
-        <v>45143</v>
+      <c r="C47" s="7">
+        <v>5.8</v>
       </c>
       <c r="D47" s="3">
         <v>19</v>
@@ -1838,8 +1837,8 @@
       <c r="E47" s="3">
         <v>86</v>
       </c>
-      <c r="F47" s="5">
-        <v>44992</v>
+      <c r="F47" s="7">
+        <v>7.3</v>
       </c>
       <c r="G47" s="3">
         <v>4</v>
@@ -1851,15 +1850,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B48" s="3">
         <v>3</v>
       </c>
-      <c r="C48" s="5">
-        <v>45142</v>
+      <c r="C48" s="7">
+        <v>4.8</v>
       </c>
       <c r="D48" s="3">
         <v>21</v>
@@ -1867,8 +1866,8 @@
       <c r="E48" s="3">
         <v>56</v>
       </c>
-      <c r="F48" s="5">
-        <v>45024</v>
+      <c r="F48" s="7">
+        <v>8.4</v>
       </c>
       <c r="G48" s="3">
         <v>3</v>
@@ -1880,15 +1879,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B49" s="3">
         <v>4</v>
       </c>
-      <c r="C49" s="5">
-        <v>45049</v>
+      <c r="C49" s="7">
+        <v>3.5</v>
       </c>
       <c r="D49" s="3">
         <v>12</v>
@@ -1896,8 +1895,8 @@
       <c r="E49" s="3">
         <v>46</v>
       </c>
-      <c r="F49" s="5">
-        <v>44994</v>
+      <c r="F49" s="7">
+        <v>9.3000000000000007</v>
       </c>
       <c r="G49" s="3">
         <v>3</v>
@@ -1909,15 +1908,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="3">
         <v>5</v>
       </c>
-      <c r="C50" s="5">
-        <v>45112</v>
+      <c r="C50" s="7">
+        <v>5.7</v>
       </c>
       <c r="D50" s="3">
         <v>14</v>
@@ -1925,8 +1924,8 @@
       <c r="E50" s="3">
         <v>74</v>
       </c>
-      <c r="F50" s="5">
-        <v>45116</v>
+      <c r="F50" s="7">
+        <v>9.6999999999999993</v>
       </c>
       <c r="G50" s="3">
         <v>3</v>
@@ -1938,15 +1937,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B51" s="3">
         <v>6</v>
       </c>
-      <c r="C51" s="5">
-        <v>45111</v>
+      <c r="C51" s="7">
+        <v>4.7</v>
       </c>
       <c r="D51" s="3">
         <v>10</v>
@@ -1954,8 +1953,8 @@
       <c r="E51" s="3">
         <v>20</v>
       </c>
-      <c r="F51" s="5">
-        <v>45113</v>
+      <c r="F51" s="7">
+        <v>6.7</v>
       </c>
       <c r="G51" s="3">
         <v>3</v>
@@ -1968,15 +1967,15 @@
       </c>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B52" s="3">
         <v>7</v>
       </c>
-      <c r="C52" s="5">
-        <v>45053</v>
+      <c r="C52" s="7">
+        <v>7.5</v>
       </c>
       <c r="D52" s="3">
         <v>22</v>
@@ -1984,8 +1983,8 @@
       <c r="E52" s="3">
         <v>66</v>
       </c>
-      <c r="F52" s="5">
-        <v>45055</v>
+      <c r="F52" s="7">
+        <v>9.5</v>
       </c>
       <c r="G52" s="3">
         <v>4</v>
@@ -2000,15 +1999,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B53" s="3">
         <v>8</v>
       </c>
-      <c r="C53" s="5">
-        <v>45081</v>
+      <c r="C53" s="7">
+        <v>4.5999999999999996</v>
       </c>
       <c r="D53" s="3">
         <v>18</v>
@@ -2016,8 +2015,8 @@
       <c r="E53" s="3">
         <v>51</v>
       </c>
-      <c r="F53" s="5">
-        <v>45118</v>
+      <c r="F53" s="7">
+        <v>11.7</v>
       </c>
       <c r="G53" s="3">
         <v>3</v>
@@ -2030,15 +2029,15 @@
       </c>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B54" s="3">
         <v>9</v>
       </c>
-      <c r="C54" s="5">
-        <v>45050</v>
+      <c r="C54" s="7">
+        <v>4.5</v>
       </c>
       <c r="D54" s="3">
         <v>17</v>
@@ -2046,7 +2045,7 @@
       <c r="E54" s="3">
         <v>68</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54" s="7">
         <v>7</v>
       </c>
       <c r="G54" s="3">
@@ -2060,15 +2059,15 @@
       </c>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B55" s="3">
         <v>10</v>
       </c>
-      <c r="C55" s="5">
-        <v>45051</v>
+      <c r="C55" s="7">
+        <v>5.5</v>
       </c>
       <c r="D55" s="3">
         <v>15</v>
@@ -2076,8 +2075,8 @@
       <c r="E55" s="3">
         <v>40</v>
       </c>
-      <c r="F55" s="5">
-        <v>44933</v>
+      <c r="F55" s="7">
+        <v>7.1</v>
       </c>
       <c r="G55" s="3">
         <v>4</v>
@@ -2089,15 +2088,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B56" s="3">
         <v>1</v>
       </c>
-      <c r="C56" s="5">
-        <v>45141</v>
+      <c r="C56" s="7">
+        <v>3.8</v>
       </c>
       <c r="D56" s="3">
         <v>9</v>
@@ -2105,8 +2104,8 @@
       <c r="E56" s="3">
         <v>23</v>
       </c>
-      <c r="F56" s="5">
-        <v>44935</v>
+      <c r="F56" s="7">
+        <v>9.1</v>
       </c>
       <c r="G56" s="3">
         <v>1</v>
@@ -2118,15 +2117,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B57" s="3">
         <v>2</v>
       </c>
-      <c r="C57" s="5">
-        <v>44928</v>
+      <c r="C57" s="7">
+        <v>2.1</v>
       </c>
       <c r="D57" s="3">
         <v>8</v>
@@ -2134,8 +2133,8 @@
       <c r="E57" s="3">
         <v>24</v>
       </c>
-      <c r="F57" s="5">
-        <v>44994</v>
+      <c r="F57" s="7">
+        <v>9.3000000000000007</v>
       </c>
       <c r="G57" s="3">
         <v>1</v>
@@ -2147,15 +2146,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B58" s="3">
         <v>3</v>
       </c>
-      <c r="C58" s="5">
-        <v>44931</v>
+      <c r="C58" s="7">
+        <v>5.0999999999999996</v>
       </c>
       <c r="D58" s="3">
         <v>13</v>
@@ -2163,8 +2162,8 @@
       <c r="E58" s="3">
         <v>70</v>
       </c>
-      <c r="F58" s="5">
-        <v>45057</v>
+      <c r="F58" s="7">
+        <v>11.5</v>
       </c>
       <c r="G58" s="3">
         <v>2</v>
@@ -2176,15 +2175,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B59" s="3">
         <v>4</v>
       </c>
-      <c r="C59" s="5">
-        <v>45049</v>
+      <c r="C59" s="7">
+        <v>3.5</v>
       </c>
       <c r="D59" s="3">
         <v>8</v>
@@ -2192,8 +2191,8 @@
       <c r="E59" s="3">
         <v>15</v>
       </c>
-      <c r="F59" s="5">
-        <v>45085</v>
+      <c r="F59" s="7">
+        <v>8.6</v>
       </c>
       <c r="G59" s="3">
         <v>2</v>
@@ -2205,14 +2204,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B60" s="3">
         <v>5</v>
       </c>
-      <c r="C60" s="6">
+      <c r="C60" s="7">
         <v>4</v>
       </c>
       <c r="D60" s="3">
@@ -2221,8 +2220,8 @@
       <c r="E60" s="3">
         <v>18</v>
       </c>
-      <c r="F60" s="5">
-        <v>45054</v>
+      <c r="F60" s="7">
+        <v>8.5</v>
       </c>
       <c r="G60" s="3">
         <v>1</v>
@@ -2234,15 +2233,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B61" s="3">
         <v>6</v>
       </c>
-      <c r="C61" s="5">
-        <v>45079</v>
+      <c r="C61" s="7">
+        <v>2.6</v>
       </c>
       <c r="D61" s="3">
         <v>12</v>
@@ -2250,8 +2249,8 @@
       <c r="E61" s="3">
         <v>64</v>
       </c>
-      <c r="F61" s="5">
-        <v>45145</v>
+      <c r="F61" s="7">
+        <v>7.8</v>
       </c>
       <c r="G61" s="3">
         <v>2</v>
@@ -2264,15 +2263,15 @@
       </c>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B62" s="3">
         <v>7</v>
       </c>
-      <c r="C62" s="5">
-        <v>45081</v>
+      <c r="C62" s="7">
+        <v>4.5999999999999996</v>
       </c>
       <c r="D62" s="3">
         <v>25</v>
@@ -2280,8 +2279,8 @@
       <c r="E62" s="3">
         <v>72</v>
       </c>
-      <c r="F62" s="5">
-        <v>45083</v>
+      <c r="F62" s="7">
+        <v>6.6</v>
       </c>
       <c r="G62" s="3">
         <v>1</v>
@@ -2294,15 +2293,15 @@
       </c>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B63" s="3">
         <v>8</v>
       </c>
-      <c r="C63" s="5">
-        <v>45081</v>
+      <c r="C63" s="7">
+        <v>4.5999999999999996</v>
       </c>
       <c r="D63" s="3">
         <v>17</v>
@@ -2310,8 +2309,8 @@
       <c r="E63" s="3">
         <v>38</v>
       </c>
-      <c r="F63" s="5">
-        <v>45053</v>
+      <c r="F63" s="7">
+        <v>7.5</v>
       </c>
       <c r="G63" s="3">
         <v>2</v>
@@ -2324,15 +2323,15 @@
       </c>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B64" s="3">
         <v>9</v>
       </c>
-      <c r="C64" s="5">
-        <v>45109</v>
+      <c r="C64" s="7">
+        <v>2.7</v>
       </c>
       <c r="D64" s="3">
         <v>9</v>
@@ -2340,8 +2339,8 @@
       <c r="E64" s="3">
         <v>18</v>
       </c>
-      <c r="F64" s="5">
-        <v>45175</v>
+      <c r="F64" s="7">
+        <v>6.9</v>
       </c>
       <c r="G64" s="3">
         <v>1</v>
@@ -2353,15 +2352,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B65" s="3">
         <v>10</v>
       </c>
-      <c r="C65" s="5">
-        <v>44933</v>
+      <c r="C65" s="7">
+        <v>7.1</v>
       </c>
       <c r="D65" s="3">
         <v>33</v>
@@ -2369,13 +2368,13 @@
       <c r="E65" s="3">
         <v>72</v>
       </c>
-      <c r="F65" s="5">
-        <v>44994</v>
+      <c r="F65" s="7">
+        <v>9.3000000000000007</v>
       </c>
       <c r="G65" s="3">
         <v>1</v>
       </c>
-      <c r="H65" s="7">
+      <c r="H65" s="5">
         <v>4248</v>
       </c>
       <c r="I65" s="3">
@@ -2383,15 +2382,15 @@
       </c>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B66" s="3">
         <v>1</v>
       </c>
-      <c r="C66" s="5">
-        <v>44931</v>
+      <c r="C66" s="7">
+        <v>5.0999999999999996</v>
       </c>
       <c r="D66" s="3">
         <v>11</v>
@@ -2399,8 +2398,8 @@
       <c r="E66" s="3">
         <v>24</v>
       </c>
-      <c r="F66" s="5">
-        <v>44936</v>
+      <c r="F66" s="7">
+        <v>10.1</v>
       </c>
       <c r="G66" s="3">
         <v>2</v>
@@ -2412,15 +2411,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B67" s="3">
         <v>2</v>
       </c>
-      <c r="C67" s="5">
-        <v>44990</v>
+      <c r="C67" s="7">
+        <v>5.3</v>
       </c>
       <c r="D67" s="3">
         <v>13</v>
@@ -2428,8 +2427,8 @@
       <c r="E67" s="3">
         <v>23</v>
       </c>
-      <c r="F67" s="5">
-        <v>44937</v>
+      <c r="F67" s="7">
+        <v>11.1</v>
       </c>
       <c r="G67" s="3">
         <v>2</v>
@@ -2441,15 +2440,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B68" s="3">
         <v>3</v>
       </c>
-      <c r="C68" s="5">
-        <v>44963</v>
+      <c r="C68" s="7">
+        <v>6.2</v>
       </c>
       <c r="D68" s="3">
         <v>10</v>
@@ -2457,8 +2456,8 @@
       <c r="E68" s="3">
         <v>38</v>
       </c>
-      <c r="F68" s="5">
-        <v>45086</v>
+      <c r="F68" s="7">
+        <v>9.6</v>
       </c>
       <c r="G68" s="3">
         <v>2</v>
@@ -2471,15 +2470,15 @@
       </c>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B69" s="3">
         <v>4</v>
       </c>
-      <c r="C69" s="5">
-        <v>45085</v>
+      <c r="C69" s="7">
+        <v>8.6</v>
       </c>
       <c r="D69" s="3">
         <v>19</v>
@@ -2487,8 +2486,8 @@
       <c r="E69" s="3">
         <v>36</v>
       </c>
-      <c r="F69" s="5">
-        <v>45177</v>
+      <c r="F69" s="7">
+        <v>8.9</v>
       </c>
       <c r="G69" s="3">
         <v>2</v>
@@ -2503,15 +2502,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B70" s="3">
         <v>5</v>
       </c>
-      <c r="C70" s="5">
-        <v>45171</v>
+      <c r="C70" s="7">
+        <v>2.9</v>
       </c>
       <c r="D70" s="3">
         <v>11</v>
@@ -2519,8 +2518,8 @@
       <c r="E70" s="3">
         <v>33</v>
       </c>
-      <c r="F70" s="5">
-        <v>45115</v>
+      <c r="F70" s="7">
+        <v>8.6999999999999993</v>
       </c>
       <c r="G70" s="3">
         <v>2</v>
@@ -2533,15 +2532,15 @@
       </c>
       <c r="J70" s="3"/>
     </row>
-    <row r="71" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B71" s="3">
         <v>6</v>
       </c>
-      <c r="C71" s="5">
-        <v>45174</v>
+      <c r="C71" s="7">
+        <v>5.9</v>
       </c>
       <c r="D71" s="3">
         <v>15</v>
@@ -2549,8 +2548,8 @@
       <c r="E71" s="3">
         <v>84</v>
       </c>
-      <c r="F71" s="5">
-        <v>45145</v>
+      <c r="F71" s="7">
+        <v>7.8</v>
       </c>
       <c r="G71" s="3">
         <v>2</v>
@@ -2565,15 +2564,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B72" s="3">
         <v>7</v>
       </c>
-      <c r="C72" s="5">
-        <v>45022</v>
+      <c r="C72" s="7">
+        <v>6.4</v>
       </c>
       <c r="D72" s="3">
         <v>13</v>
@@ -2581,8 +2580,8 @@
       <c r="E72" s="3">
         <v>23</v>
       </c>
-      <c r="F72" s="5">
-        <v>45114</v>
+      <c r="F72" s="7">
+        <v>7.7</v>
       </c>
       <c r="G72" s="3">
         <v>2</v>
@@ -2597,15 +2596,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B73" s="3">
         <v>8</v>
       </c>
-      <c r="C73" s="5">
-        <v>45113</v>
+      <c r="C73" s="7">
+        <v>6.7</v>
       </c>
       <c r="D73" s="3">
         <v>13</v>
@@ -2613,8 +2612,8 @@
       <c r="E73" s="3">
         <v>47</v>
       </c>
-      <c r="F73" s="5">
-        <v>44935</v>
+      <c r="F73" s="7">
+        <v>9.1</v>
       </c>
       <c r="G73" s="3">
         <v>2</v>
@@ -2629,15 +2628,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B74" s="3">
         <v>9</v>
       </c>
-      <c r="C74" s="5">
-        <v>44990</v>
+      <c r="C74" s="7">
+        <v>5.3</v>
       </c>
       <c r="D74" s="3">
         <v>14</v>
@@ -2645,7 +2644,7 @@
       <c r="E74" s="3">
         <v>40</v>
       </c>
-      <c r="F74" s="3">
+      <c r="F74" s="7">
         <v>9</v>
       </c>
       <c r="G74" s="3">
@@ -2658,15 +2657,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B75" s="3">
         <v>10</v>
       </c>
-      <c r="C75" s="5">
-        <v>45082</v>
+      <c r="C75" s="7">
+        <v>5.6</v>
       </c>
       <c r="D75" s="3">
         <v>22</v>
@@ -2674,8 +2673,8 @@
       <c r="E75" s="3">
         <v>88</v>
       </c>
-      <c r="F75" s="5">
-        <v>45115</v>
+      <c r="F75" s="7">
+        <v>8.6999999999999993</v>
       </c>
       <c r="G75" s="3">
         <v>2</v>
@@ -2685,8 +2684,8 @@
       </c>
       <c r="J75" s="3"/>
     </row>
-    <row r="76" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="77" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="76" spans="1:10" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="77" spans="1:10" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added for loop for shapiro wilk
</commit_message>
<xml_diff>
--- a/data/arabidopsis_data.xlsx
+++ b/data/arabidopsis_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nineluijendijk/evolutionarybiology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE69859-4589-DB46-8F46-1730AC25CD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DECA4C-FEB1-F349-A9C2-9422D0539AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="43">
   <si>
     <t>Group</t>
   </si>
@@ -144,14 +144,21 @@
   </si>
   <si>
     <t>nods forming</t>
+  </si>
+  <si>
+    <t>Missing the wet weight of S8 - 10</t>
+  </si>
+  <si>
+    <t>Missing the number of leaves before S3 - 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -231,9 +238,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,8 +461,8 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -483,7 +490,7 @@
       <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -506,7 +513,7 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>4.3</v>
       </c>
       <c r="D2" s="3">
@@ -515,7 +522,7 @@
       <c r="E2" s="3">
         <v>28</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>9.6999999999999993</v>
       </c>
       <c r="G2" s="3">
@@ -535,7 +542,7 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>8</v>
       </c>
       <c r="D3" s="3">
@@ -544,7 +551,7 @@
       <c r="E3" s="3">
         <v>27</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>9.5</v>
       </c>
       <c r="G3" s="3">
@@ -565,7 +572,7 @@
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>2</v>
       </c>
       <c r="D4" s="3">
@@ -574,7 +581,7 @@
       <c r="E4" s="3">
         <v>12</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>9.4</v>
       </c>
       <c r="G4" s="3">
@@ -594,7 +601,7 @@
       <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>3.1</v>
       </c>
       <c r="D5" s="3">
@@ -603,7 +610,7 @@
       <c r="E5" s="3">
         <v>12</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>6.7</v>
       </c>
       <c r="G5" s="3">
@@ -623,7 +630,7 @@
       <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>4.5</v>
       </c>
       <c r="D6" s="3">
@@ -632,7 +639,7 @@
       <c r="E6" s="3">
         <v>22</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>11.3</v>
       </c>
       <c r="G6" s="3">
@@ -653,7 +660,7 @@
       <c r="B7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>6.9</v>
       </c>
       <c r="D7" s="3">
@@ -662,7 +669,7 @@
       <c r="E7" s="3">
         <v>35</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>10.7</v>
       </c>
       <c r="G7" s="3">
@@ -682,7 +689,7 @@
       <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>4.5</v>
       </c>
       <c r="D8" s="3">
@@ -691,7 +698,7 @@
       <c r="E8" s="3">
         <v>40</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>10.199999999999999</v>
       </c>
       <c r="G8" s="3">
@@ -711,7 +718,7 @@
       <c r="B9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>2.1</v>
       </c>
       <c r="D9" s="3">
@@ -720,7 +727,7 @@
       <c r="E9" s="3">
         <v>23</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>9.8000000000000007</v>
       </c>
       <c r="G9" s="3">
@@ -740,7 +747,7 @@
       <c r="B10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>0.8</v>
       </c>
       <c r="D10" s="3">
@@ -749,7 +756,7 @@
       <c r="E10" s="3">
         <v>20</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>10.6</v>
       </c>
       <c r="G10" s="3">
@@ -769,7 +776,7 @@
       <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>2.8</v>
       </c>
       <c r="D11" s="3">
@@ -778,7 +785,7 @@
       <c r="E11" s="3">
         <v>25</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>8.5</v>
       </c>
       <c r="G11" s="3">
@@ -799,7 +806,7 @@
       <c r="B12" s="3">
         <v>1</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>5.8</v>
       </c>
       <c r="D12" s="3">
@@ -808,7 +815,7 @@
       <c r="E12" s="3">
         <v>23</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>10</v>
       </c>
       <c r="G12" s="3">
@@ -828,7 +835,7 @@
       <c r="B13" s="3">
         <v>2</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>5.7</v>
       </c>
       <c r="D13" s="3">
@@ -837,7 +844,7 @@
       <c r="E13" s="3">
         <v>30</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>7</v>
       </c>
       <c r="G13" s="3">
@@ -858,7 +865,7 @@
       <c r="B14" s="3">
         <v>3</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>5.7</v>
       </c>
       <c r="D14" s="3">
@@ -867,7 +874,7 @@
       <c r="E14" s="3">
         <v>30</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>10.4</v>
       </c>
       <c r="G14" s="3">
@@ -888,7 +895,7 @@
       <c r="B15" s="3">
         <v>4</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>7.8</v>
       </c>
       <c r="D15" s="3">
@@ -897,7 +904,7 @@
       <c r="E15" s="3">
         <v>44</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>10.7</v>
       </c>
       <c r="G15" s="3">
@@ -918,7 +925,7 @@
       <c r="B16" s="3">
         <v>5</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>4.5</v>
       </c>
       <c r="D16" s="3">
@@ -927,7 +934,7 @@
       <c r="E16" s="3">
         <v>42</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>6.8</v>
       </c>
       <c r="G16" s="3">
@@ -948,7 +955,7 @@
       <c r="B17" s="3">
         <v>6</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>1</v>
       </c>
       <c r="D17" s="3">
@@ -957,7 +964,7 @@
       <c r="E17" s="3">
         <v>15</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>3.5</v>
       </c>
       <c r="G17" s="3">
@@ -978,7 +985,7 @@
       <c r="B18" s="3">
         <v>7</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>4.4000000000000004</v>
       </c>
       <c r="D18" s="3">
@@ -987,7 +994,7 @@
       <c r="E18" s="3">
         <v>42</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>9</v>
       </c>
       <c r="G18" s="3">
@@ -1007,7 +1014,7 @@
       <c r="B19" s="3">
         <v>8</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>6.2</v>
       </c>
       <c r="D19" s="3">
@@ -1016,7 +1023,7 @@
       <c r="E19" s="3">
         <v>33</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>8.5</v>
       </c>
       <c r="G19" s="3">
@@ -1037,7 +1044,7 @@
       <c r="B20" s="3">
         <v>9</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>4.0999999999999996</v>
       </c>
       <c r="D20" s="3">
@@ -1046,7 +1053,7 @@
       <c r="E20" s="3">
         <v>23</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>11</v>
       </c>
       <c r="G20" s="3">
@@ -1066,7 +1073,7 @@
       <c r="B21" s="3">
         <v>10</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>6.9</v>
       </c>
       <c r="D21" s="3">
@@ -1075,7 +1082,7 @@
       <c r="E21" s="3">
         <v>32</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>11.3</v>
       </c>
       <c r="G21" s="3">
@@ -1095,7 +1102,7 @@
       <c r="B22" s="3">
         <v>1</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>2.2000000000000002</v>
       </c>
       <c r="D22" s="3">
@@ -1104,7 +1111,7 @@
       <c r="E22" s="3">
         <v>38</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>9.5</v>
       </c>
       <c r="G22" s="3">
@@ -1124,7 +1131,7 @@
       <c r="B23" s="3">
         <v>2</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>3.8</v>
       </c>
       <c r="D23" s="3">
@@ -1133,7 +1140,7 @@
       <c r="E23" s="3">
         <v>22</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>7.4</v>
       </c>
       <c r="G23" s="3">
@@ -1153,7 +1160,7 @@
       <c r="B24" s="3">
         <v>3</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>6.6</v>
       </c>
       <c r="D24" s="3">
@@ -1162,7 +1169,7 @@
       <c r="E24" s="3">
         <v>48</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>11.4</v>
       </c>
       <c r="G24" s="3">
@@ -1182,13 +1189,13 @@
       <c r="B25" s="3">
         <v>4</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>5.5</v>
       </c>
       <c r="E25" s="3">
         <v>64</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>9.5</v>
       </c>
       <c r="G25" s="3">
@@ -1209,7 +1216,7 @@
       <c r="B26" s="3">
         <v>5</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>2.6</v>
       </c>
       <c r="D26" s="3">
@@ -1218,7 +1225,7 @@
       <c r="E26" s="3">
         <v>24</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>10.6</v>
       </c>
       <c r="G26" s="3">
@@ -1238,7 +1245,7 @@
       <c r="B27" s="3">
         <v>6</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>5.0999999999999996</v>
       </c>
       <c r="D27" s="3">
@@ -1247,7 +1254,7 @@
       <c r="E27" s="3">
         <v>34</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>12.5</v>
       </c>
       <c r="G27" s="3">
@@ -1267,7 +1274,7 @@
       <c r="B28" s="3">
         <v>7</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>2.4</v>
       </c>
       <c r="D28" s="3">
@@ -1276,7 +1283,7 @@
       <c r="E28" s="3">
         <v>24</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <v>8</v>
       </c>
       <c r="G28" s="3">
@@ -1296,7 +1303,7 @@
       <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>4.2</v>
       </c>
       <c r="D29" s="3">
@@ -1305,7 +1312,7 @@
       <c r="E29" s="3">
         <v>32</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>6</v>
       </c>
       <c r="G29" s="3">
@@ -1325,7 +1332,7 @@
       <c r="B30" s="3">
         <v>2</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>4.5999999999999996</v>
       </c>
       <c r="D30" s="3">
@@ -1334,7 +1341,7 @@
       <c r="E30" s="3">
         <v>68</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>9.5</v>
       </c>
       <c r="G30" s="3">
@@ -1354,7 +1361,7 @@
       <c r="B31" s="3">
         <v>3</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>3.6</v>
       </c>
       <c r="D31" s="3">
@@ -1363,7 +1370,7 @@
       <c r="E31" s="3">
         <v>18</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>9.6999999999999993</v>
       </c>
       <c r="G31" s="3">
@@ -1383,7 +1390,7 @@
       <c r="B32" s="3">
         <v>4</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>7.3</v>
       </c>
       <c r="D32" s="3">
@@ -1392,7 +1399,7 @@
       <c r="E32" s="3">
         <v>36</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>12.4</v>
       </c>
       <c r="G32" s="3">
@@ -1412,7 +1419,7 @@
       <c r="B33" s="3">
         <v>5</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <v>5.6</v>
       </c>
       <c r="D33" s="3">
@@ -1421,7 +1428,7 @@
       <c r="E33" s="3">
         <v>24</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="6">
         <v>10.7</v>
       </c>
       <c r="G33" s="3">
@@ -1441,7 +1448,7 @@
       <c r="B34" s="3">
         <v>6</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>4.4000000000000004</v>
       </c>
       <c r="D34" s="3">
@@ -1450,7 +1457,7 @@
       <c r="E34" s="3">
         <v>32</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>10</v>
       </c>
       <c r="G34" s="3">
@@ -1470,7 +1477,7 @@
       <c r="B35" s="3">
         <v>7</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>3.9</v>
       </c>
       <c r="D35" s="3">
@@ -1479,7 +1486,7 @@
       <c r="E35" s="3">
         <v>54</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="6">
         <v>8.1</v>
       </c>
       <c r="G35" s="3">
@@ -1499,7 +1506,7 @@
       <c r="B36" s="3">
         <v>8</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>6.7</v>
       </c>
       <c r="D36" s="3">
@@ -1508,7 +1515,7 @@
       <c r="E36" s="3">
         <v>32</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="6">
         <v>9.5</v>
       </c>
       <c r="G36" s="3">
@@ -1528,7 +1535,7 @@
       <c r="B37" s="3">
         <v>1</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="6">
         <v>4.5999999999999996</v>
       </c>
       <c r="D37" s="3">
@@ -1537,7 +1544,7 @@
       <c r="E37" s="3">
         <v>82</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>7.6</v>
       </c>
       <c r="G37" s="3">
@@ -1557,7 +1564,7 @@
       <c r="B38" s="3">
         <v>2</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>8.6</v>
       </c>
       <c r="D38" s="3">
@@ -1566,7 +1573,7 @@
       <c r="E38" s="3">
         <v>31</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="6">
         <v>9.4</v>
       </c>
       <c r="G38" s="3">
@@ -1587,7 +1594,7 @@
       <c r="B39" s="3">
         <v>3</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <v>6.3</v>
       </c>
       <c r="D39" s="3">
@@ -1596,7 +1603,7 @@
       <c r="E39" s="3">
         <v>37</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="6">
         <v>9.6999999999999993</v>
       </c>
       <c r="G39" s="3">
@@ -1616,7 +1623,7 @@
       <c r="B40" s="3">
         <v>4</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="6">
         <v>5</v>
       </c>
       <c r="D40" s="3">
@@ -1625,7 +1632,7 @@
       <c r="E40" s="3">
         <v>106</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="6">
         <v>7.5</v>
       </c>
       <c r="G40" s="3">
@@ -1648,7 +1655,7 @@
       <c r="B41" s="3">
         <v>5</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="6">
         <v>5</v>
       </c>
       <c r="D41" s="3">
@@ -1657,7 +1664,7 @@
       <c r="E41" s="3">
         <v>34</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="6">
         <v>10.199999999999999</v>
       </c>
       <c r="G41" s="3">
@@ -1678,7 +1685,7 @@
       <c r="B42" s="3">
         <v>6</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="6">
         <v>6</v>
       </c>
       <c r="D42" s="3">
@@ -1687,7 +1694,7 @@
       <c r="E42" s="3">
         <v>70</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="6">
         <v>10</v>
       </c>
       <c r="G42" s="3">
@@ -1708,7 +1715,7 @@
       <c r="B43" s="3">
         <v>7</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="6">
         <v>5.7</v>
       </c>
       <c r="D43" s="3">
@@ -1717,7 +1724,7 @@
       <c r="E43" s="3">
         <v>98</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="6">
         <v>8.3000000000000007</v>
       </c>
       <c r="G43" s="3">
@@ -1738,7 +1745,7 @@
       <c r="B44" s="3">
         <v>8</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="6">
         <v>4</v>
       </c>
       <c r="D44" s="3">
@@ -1747,7 +1754,7 @@
       <c r="E44" s="3">
         <v>34</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="6">
         <v>9.9</v>
       </c>
       <c r="G44" s="3">
@@ -1767,7 +1774,7 @@
       <c r="B45" s="3">
         <v>9</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="6">
         <v>5.6</v>
       </c>
       <c r="D45" s="3">
@@ -1776,7 +1783,7 @@
       <c r="E45" s="3">
         <v>70</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="6">
         <v>11.1</v>
       </c>
       <c r="G45" s="3">
@@ -1799,7 +1806,7 @@
       <c r="B46" s="3">
         <v>1</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="6">
         <v>5.0999999999999996</v>
       </c>
       <c r="D46" s="3">
@@ -1808,7 +1815,7 @@
       <c r="E46" s="3">
         <v>98</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="6">
         <v>8.1999999999999993</v>
       </c>
       <c r="G46" s="3">
@@ -1828,7 +1835,7 @@
       <c r="B47" s="3">
         <v>2</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <v>5.8</v>
       </c>
       <c r="D47" s="3">
@@ -1837,7 +1844,7 @@
       <c r="E47" s="3">
         <v>86</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="6">
         <v>7.3</v>
       </c>
       <c r="G47" s="3">
@@ -1857,7 +1864,7 @@
       <c r="B48" s="3">
         <v>3</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="6">
         <v>4.8</v>
       </c>
       <c r="D48" s="3">
@@ -1866,7 +1873,7 @@
       <c r="E48" s="3">
         <v>56</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="6">
         <v>8.4</v>
       </c>
       <c r="G48" s="3">
@@ -1886,7 +1893,7 @@
       <c r="B49" s="3">
         <v>4</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="6">
         <v>3.5</v>
       </c>
       <c r="D49" s="3">
@@ -1895,7 +1902,7 @@
       <c r="E49" s="3">
         <v>46</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F49" s="6">
         <v>9.3000000000000007</v>
       </c>
       <c r="G49" s="3">
@@ -1915,7 +1922,7 @@
       <c r="B50" s="3">
         <v>5</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="6">
         <v>5.7</v>
       </c>
       <c r="D50" s="3">
@@ -1924,7 +1931,7 @@
       <c r="E50" s="3">
         <v>74</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F50" s="6">
         <v>9.6999999999999993</v>
       </c>
       <c r="G50" s="3">
@@ -1944,7 +1951,7 @@
       <c r="B51" s="3">
         <v>6</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="6">
         <v>4.7</v>
       </c>
       <c r="D51" s="3">
@@ -1953,7 +1960,7 @@
       <c r="E51" s="3">
         <v>20</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F51" s="6">
         <v>6.7</v>
       </c>
       <c r="G51" s="3">
@@ -1974,7 +1981,7 @@
       <c r="B52" s="3">
         <v>7</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="6">
         <v>7.5</v>
       </c>
       <c r="D52" s="3">
@@ -1983,7 +1990,7 @@
       <c r="E52" s="3">
         <v>66</v>
       </c>
-      <c r="F52" s="7">
+      <c r="F52" s="6">
         <v>9.5</v>
       </c>
       <c r="G52" s="3">
@@ -2006,7 +2013,7 @@
       <c r="B53" s="3">
         <v>8</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="6">
         <v>4.5999999999999996</v>
       </c>
       <c r="D53" s="3">
@@ -2015,7 +2022,7 @@
       <c r="E53" s="3">
         <v>51</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F53" s="6">
         <v>11.7</v>
       </c>
       <c r="G53" s="3">
@@ -2036,7 +2043,7 @@
       <c r="B54" s="3">
         <v>9</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="6">
         <v>4.5</v>
       </c>
       <c r="D54" s="3">
@@ -2045,7 +2052,7 @@
       <c r="E54" s="3">
         <v>68</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F54" s="6">
         <v>7</v>
       </c>
       <c r="G54" s="3">
@@ -2066,7 +2073,7 @@
       <c r="B55" s="3">
         <v>10</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="6">
         <v>5.5</v>
       </c>
       <c r="D55" s="3">
@@ -2075,7 +2082,7 @@
       <c r="E55" s="3">
         <v>40</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F55" s="6">
         <v>7.1</v>
       </c>
       <c r="G55" s="3">
@@ -2095,7 +2102,7 @@
       <c r="B56" s="3">
         <v>1</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="6">
         <v>3.8</v>
       </c>
       <c r="D56" s="3">
@@ -2104,7 +2111,7 @@
       <c r="E56" s="3">
         <v>23</v>
       </c>
-      <c r="F56" s="7">
+      <c r="F56" s="6">
         <v>9.1</v>
       </c>
       <c r="G56" s="3">
@@ -2124,7 +2131,7 @@
       <c r="B57" s="3">
         <v>2</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="6">
         <v>2.1</v>
       </c>
       <c r="D57" s="3">
@@ -2133,7 +2140,7 @@
       <c r="E57" s="3">
         <v>24</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F57" s="6">
         <v>9.3000000000000007</v>
       </c>
       <c r="G57" s="3">
@@ -2153,7 +2160,7 @@
       <c r="B58" s="3">
         <v>3</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="6">
         <v>5.0999999999999996</v>
       </c>
       <c r="D58" s="3">
@@ -2162,7 +2169,7 @@
       <c r="E58" s="3">
         <v>70</v>
       </c>
-      <c r="F58" s="7">
+      <c r="F58" s="6">
         <v>11.5</v>
       </c>
       <c r="G58" s="3">
@@ -2182,7 +2189,7 @@
       <c r="B59" s="3">
         <v>4</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="6">
         <v>3.5</v>
       </c>
       <c r="D59" s="3">
@@ -2191,7 +2198,7 @@
       <c r="E59" s="3">
         <v>15</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F59" s="6">
         <v>8.6</v>
       </c>
       <c r="G59" s="3">
@@ -2211,7 +2218,7 @@
       <c r="B60" s="3">
         <v>5</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="6">
         <v>4</v>
       </c>
       <c r="D60" s="3">
@@ -2220,7 +2227,7 @@
       <c r="E60" s="3">
         <v>18</v>
       </c>
-      <c r="F60" s="7">
+      <c r="F60" s="6">
         <v>8.5</v>
       </c>
       <c r="G60" s="3">
@@ -2240,7 +2247,7 @@
       <c r="B61" s="3">
         <v>6</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="6">
         <v>2.6</v>
       </c>
       <c r="D61" s="3">
@@ -2249,7 +2256,7 @@
       <c r="E61" s="3">
         <v>64</v>
       </c>
-      <c r="F61" s="7">
+      <c r="F61" s="6">
         <v>7.8</v>
       </c>
       <c r="G61" s="3">
@@ -2270,7 +2277,7 @@
       <c r="B62" s="3">
         <v>7</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="6">
         <v>4.5999999999999996</v>
       </c>
       <c r="D62" s="3">
@@ -2279,7 +2286,7 @@
       <c r="E62" s="3">
         <v>72</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F62" s="6">
         <v>6.6</v>
       </c>
       <c r="G62" s="3">
@@ -2300,7 +2307,7 @@
       <c r="B63" s="3">
         <v>8</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="6">
         <v>4.5999999999999996</v>
       </c>
       <c r="D63" s="3">
@@ -2309,7 +2316,7 @@
       <c r="E63" s="3">
         <v>38</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F63" s="6">
         <v>7.5</v>
       </c>
       <c r="G63" s="3">
@@ -2330,7 +2337,7 @@
       <c r="B64" s="3">
         <v>9</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="6">
         <v>2.7</v>
       </c>
       <c r="D64" s="3">
@@ -2339,7 +2346,7 @@
       <c r="E64" s="3">
         <v>18</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F64" s="6">
         <v>6.9</v>
       </c>
       <c r="G64" s="3">
@@ -2359,7 +2366,7 @@
       <c r="B65" s="3">
         <v>10</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="6">
         <v>7.1</v>
       </c>
       <c r="D65" s="3">
@@ -2368,14 +2375,14 @@
       <c r="E65" s="3">
         <v>72</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F65" s="6">
         <v>9.3000000000000007</v>
       </c>
       <c r="G65" s="3">
         <v>1</v>
       </c>
-      <c r="H65" s="5">
-        <v>4248</v>
+      <c r="H65" s="7">
+        <v>4.2480000000000002</v>
       </c>
       <c r="I65" s="3">
         <v>2</v>
@@ -2389,7 +2396,7 @@
       <c r="B66" s="3">
         <v>1</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="6">
         <v>5.0999999999999996</v>
       </c>
       <c r="D66" s="3">
@@ -2398,7 +2405,7 @@
       <c r="E66" s="3">
         <v>24</v>
       </c>
-      <c r="F66" s="7">
+      <c r="F66" s="6">
         <v>10.1</v>
       </c>
       <c r="G66" s="3">
@@ -2418,7 +2425,7 @@
       <c r="B67" s="3">
         <v>2</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="6">
         <v>5.3</v>
       </c>
       <c r="D67" s="3">
@@ -2427,7 +2434,7 @@
       <c r="E67" s="3">
         <v>23</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F67" s="6">
         <v>11.1</v>
       </c>
       <c r="G67" s="3">
@@ -2447,7 +2454,7 @@
       <c r="B68" s="3">
         <v>3</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="6">
         <v>6.2</v>
       </c>
       <c r="D68" s="3">
@@ -2456,7 +2463,7 @@
       <c r="E68" s="3">
         <v>38</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F68" s="6">
         <v>9.6</v>
       </c>
       <c r="G68" s="3">
@@ -2477,7 +2484,7 @@
       <c r="B69" s="3">
         <v>4</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="6">
         <v>8.6</v>
       </c>
       <c r="D69" s="3">
@@ -2486,7 +2493,7 @@
       <c r="E69" s="3">
         <v>36</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F69" s="6">
         <v>8.9</v>
       </c>
       <c r="G69" s="3">
@@ -2509,7 +2516,7 @@
       <c r="B70" s="3">
         <v>5</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="6">
         <v>2.9</v>
       </c>
       <c r="D70" s="3">
@@ -2518,7 +2525,7 @@
       <c r="E70" s="3">
         <v>33</v>
       </c>
-      <c r="F70" s="7">
+      <c r="F70" s="6">
         <v>8.6999999999999993</v>
       </c>
       <c r="G70" s="3">
@@ -2539,7 +2546,7 @@
       <c r="B71" s="3">
         <v>6</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="6">
         <v>5.9</v>
       </c>
       <c r="D71" s="3">
@@ -2548,7 +2555,7 @@
       <c r="E71" s="3">
         <v>84</v>
       </c>
-      <c r="F71" s="7">
+      <c r="F71" s="6">
         <v>7.8</v>
       </c>
       <c r="G71" s="3">
@@ -2571,7 +2578,7 @@
       <c r="B72" s="3">
         <v>7</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="6">
         <v>6.4</v>
       </c>
       <c r="D72" s="3">
@@ -2580,7 +2587,7 @@
       <c r="E72" s="3">
         <v>23</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F72" s="6">
         <v>7.7</v>
       </c>
       <c r="G72" s="3">
@@ -2603,7 +2610,7 @@
       <c r="B73" s="3">
         <v>8</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="6">
         <v>6.7</v>
       </c>
       <c r="D73" s="3">
@@ -2612,7 +2619,7 @@
       <c r="E73" s="3">
         <v>47</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F73" s="6">
         <v>9.1</v>
       </c>
       <c r="G73" s="3">
@@ -2635,7 +2642,7 @@
       <c r="B74" s="3">
         <v>9</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="6">
         <v>5.3</v>
       </c>
       <c r="D74" s="3">
@@ -2644,7 +2651,7 @@
       <c r="E74" s="3">
         <v>40</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F74" s="6">
         <v>9</v>
       </c>
       <c r="G74" s="3">
@@ -2664,7 +2671,7 @@
       <c r="B75" s="3">
         <v>10</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="6">
         <v>5.6</v>
       </c>
       <c r="D75" s="3">
@@ -2673,7 +2680,7 @@
       <c r="E75" s="3">
         <v>88</v>
       </c>
-      <c r="F75" s="7">
+      <c r="F75" s="6">
         <v>8.6999999999999993</v>
       </c>
       <c r="G75" s="3">
@@ -2694,10 +2701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC43C862-5980-D541-8E0F-338CE248DD0C}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2783,12 +2790,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
markdown complete for now
</commit_message>
<xml_diff>
--- a/data/arabidopsis_data.xlsx
+++ b/data/arabidopsis_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nineluijendijk/evolutionarybiology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DECA4C-FEB1-F349-A9C2-9422D0539AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233A5222-BCE8-494D-91FD-592F10BBBBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
   <si>
     <t>Group</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Missing the number of leaves before S3 - 4</t>
+  </si>
+  <si>
+    <t>Wet weight is measured in grams</t>
+  </si>
+  <si>
+    <t>Leaf length is measured in centimeters</t>
   </si>
 </sst>
 </file>
@@ -158,7 +164,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -240,7 +246,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,8 +467,8 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2701,10 +2707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC43C862-5980-D541-8E0F-338CE248DD0C}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2808,6 +2814,16 @@
         <v>42</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>